<commit_message>
New Assets and SQL Enhancements
New Assets and SQL Enhancements
</commit_message>
<xml_diff>
--- a/PED/DB Schema.xlsx
+++ b/PED/DB Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thermofisher-my.sharepoint.com/personal/manuel_mora_thermofisher_com/Documents/PI/GitHub/PED/PED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c09c5e7837251f87/M3 - Carrer Path/UFidelitas/2024/Cuatrimestre 2/Estructuras de datos/PED/PED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B09DD6A-E123-4E1F-98C9-9B752D68484D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{9B09DD6A-E123-4E1F-98C9-9B752D68484D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB757ABD-E301-4091-A7D6-46F295FAD394}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A78AA3C-F35A-4710-B4DF-EC8C8324D33A}"/>
+    <workbookView xWindow="23490" yWindow="0" windowWidth="5415" windowHeight="15585" xr2:uid="{7A78AA3C-F35A-4710-B4DF-EC8C8324D33A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>BankInfo</t>
   </si>
@@ -140,7 +140,10 @@
     <t>uLastLogin</t>
   </si>
   <si>
-    <t>tProcedure</t>
+    <t>tClientID</t>
+  </si>
+  <si>
+    <t>bDispensers</t>
   </si>
 </sst>
 </file>
@@ -268,15 +271,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -288,9 +288,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -300,15 +297,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,10 +363,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -407,19 +395,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FECD05F8-19E9-430F-A7FD-BBF8754F7512}" name="Table1" displayName="Table1" ref="C2:D7" totalsRowShown="0" headerRowDxfId="22" dataDxfId="23">
-  <autoFilter ref="C2:D7" xr:uid="{FECD05F8-19E9-430F-A7FD-BBF8754F7512}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FECD05F8-19E9-430F-A7FD-BBF8754F7512}" name="Table1" displayName="Table1" ref="C2:D8" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="C2:D8" xr:uid="{FECD05F8-19E9-430F-A7FD-BBF8754F7512}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F21FB140-CE50-45DA-B558-8D11B7E501BE}" name="Col Name" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{297AD780-F414-4DF2-B85A-DBBED248DE04}" name="Data Type" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{F21FB140-CE50-45DA-B558-8D11B7E501BE}" name="Col Name" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{297AD780-F414-4DF2-B85A-DBBED248DE04}" name="Data Type" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{469C674F-E168-4195-9A69-FBFF7FAE3FF6}" name="Table13" displayName="Table13" ref="C11:D15" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="C11:D15" xr:uid="{469C674F-E168-4195-9A69-FBFF7FAE3FF6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{469C674F-E168-4195-9A69-FBFF7FAE3FF6}" name="Table13" displayName="Table13" ref="C10:D14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="C10:D14" xr:uid="{469C674F-E168-4195-9A69-FBFF7FAE3FF6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9FC2AECC-76AD-4A92-91AB-EB4C13B8560E}" name="Col Name" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{A67F790D-9D00-460A-9172-A62EDFC35F5B}" name="Data Type" dataDxfId="16"/>
@@ -440,8 +428,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFCC554-0789-4406-B388-E12D431488E9}" name="Table135" displayName="Table135" ref="K11:L16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="K11:L16" xr:uid="{ACFCC554-0789-4406-B388-E12D431488E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFCC554-0789-4406-B388-E12D431488E9}" name="Table135" displayName="Table135" ref="K10:L15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="K10:L15" xr:uid="{ACFCC554-0789-4406-B388-E12D431488E9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{25FDBE18-1F52-434B-9940-5CBF34FC884E}" name="Col Name" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{EDC14F33-C171-428C-9DBB-66D973A4EB69}" name="Data Type" dataDxfId="8"/>
@@ -451,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{65094B61-AEEF-46D2-AFC2-5A0EFE6B4BAF}" name="Table1356" displayName="Table1356" ref="C18:D25" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="C18:D25" xr:uid="{65094B61-AEEF-46D2-AFC2-5A0EFE6B4BAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{65094B61-AEEF-46D2-AFC2-5A0EFE6B4BAF}" name="Table1356" displayName="Table1356" ref="C17:D24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="C17:D24" xr:uid="{65094B61-AEEF-46D2-AFC2-5A0EFE6B4BAF}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{41717D0F-E7E1-4A09-82F8-5CEF0148F32D}" name="Col Name" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{21992DE5-1400-4FD3-8F09-CD2AE3BEA938}" name="Data Type" dataDxfId="4"/>
@@ -789,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB249E45-C7B8-4C39-A3A2-5B59DC719EF3}">
-  <dimension ref="B1:L26"/>
+  <dimension ref="B1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,6 +789,7 @@
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -808,320 +797,328 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="3" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="2"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="2"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="3" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="3" t="s">
+      <c r="J6" s="4"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4"/>
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="3" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="6"/>
-      <c r="C7" s="3" t="s">
+      <c r="J7" s="5"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="5"/>
+      <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="3" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="12"/>
-      <c r="G8" s="3" t="s">
+    </row>
+    <row r="9" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="7"/>
+      <c r="G9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F9" s="12"/>
-      <c r="G9" s="7" t="s">
+    <row r="10" spans="2:12" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="12"/>
-      <c r="G10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="2:12" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="J10" s="3"/>
+      <c r="K10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="L10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="7" t="s">
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="4"/>
-      <c r="K11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="7" t="s">
+      <c r="K11" s="2"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="2"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="J13" s="4"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="8"/>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="5"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:4" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="10"/>
-      <c r="C15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J16" s="6"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:4" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="B21" s="4"/>
+      <c r="C21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
-      <c r="C24" s="7" t="s">
-        <v>32</v>
+      <c r="C24" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="6"/>
-      <c r="C25" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="J2:J7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="J11:J16"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="J10:J15"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B17:B24"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="F2:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="6">

</xml_diff>

<commit_message>
SQL and GUI changes
</commit_message>
<xml_diff>
--- a/PED/DB Schema.xlsx
+++ b/PED/DB Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c09c5e7837251f87/M3 - Carrer Path/UFidelitas/2024/Cuatrimestre 2/Estructuras de datos/PED/PED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{9B09DD6A-E123-4E1F-98C9-9B752D68484D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23DD0360-EA31-4BC0-9868-8567BE5971A0}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{9B09DD6A-E123-4E1F-98C9-9B752D68484D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F1B7D5B-C983-4F1D-AC56-B4383CB39030}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A78AA3C-F35A-4710-B4DF-EC8C8324D33A}"/>
   </bookViews>
@@ -783,7 +783,7 @@
   <dimension ref="B1:L26"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,12 +1125,12 @@
     <row r="26" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B17:B25"/>
     <mergeCell ref="J2:J7"/>
     <mergeCell ref="J10:J15"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="F2:F12"/>
-    <mergeCell ref="B17:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="6">

</xml_diff>